<commit_message>
sn: prepared Septembre data.
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Senegal/septembre 2021/sn_lf_pretas_1_sites_202109.xlsx
+++ b/LF/PreTAS/Senegal/septembre 2021/sn_lf_pretas_1_sites_202109.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\PreTAS\Senegal\aout 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\PreTAS\Senegal\septembre 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96780CF4-57AA-436E-AFA4-DC648D6A9131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7544137B-F94D-4A88-AE03-FAC5FFE87501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13" yWindow="13" windowWidth="25587" windowHeight="13787" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -578,10 +578,10 @@
     <t>Sindialon</t>
   </si>
   <si>
-    <t>(Août 2021) 1. Pre-TAS FL - Formulaire Site</t>
-  </si>
-  <si>
-    <t>sn_lf_pretas_1_sites_202108</t>
+    <t>sn_lf_pretas_1_sites_202109</t>
+  </si>
+  <si>
+    <t>(Septembre 2021) 1. Pre-TAS FL - Formulaire Site</t>
   </si>
 </sst>
 </file>
@@ -3993,7 +3993,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
@@ -4019,10 +4019,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" t="s">
         <v>182</v>
-      </c>
-      <c r="B2" t="s">
-        <v>183</v>
       </c>
       <c r="C2">
         <v>20210722</v>

</xml_diff>